<commit_message>
Few tweaks to the student plan
</commit_message>
<xml_diff>
--- a/web/templates/studentplan.xlsx
+++ b/web/templates/studentplan.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenceslaus/PhpstormProjects/arina/web/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6A577A-57F7-A44D-9C45-8DC80B4278F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345AEFC1-6349-0046-BC6E-DE707E589171}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$L$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$N$34</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>ЗАТВЕРДЖУЮ</t>
   </si>
@@ -40,21 +40,12 @@
     <t>ІНДИВІДУАЛЬНИЙ НАВЧАЛЬНИЙ ПЛАН</t>
   </si>
   <si>
-    <t>на Рік/Рік</t>
-  </si>
-  <si>
     <t>Студент</t>
   </si>
   <si>
-    <t>Студент:</t>
-  </si>
-  <si>
     <t>Відділення:</t>
   </si>
   <si>
-    <t>Спеціальність/Освітня программа:</t>
-  </si>
-  <si>
     <t>Форма навчання: денна</t>
   </si>
   <si>
@@ -83,6 +74,24 @@
   </si>
   <si>
     <t>Дисципліни за вибором студента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Освітній рівень: </t>
+  </si>
+  <si>
+    <t>Спеціальність:</t>
+  </si>
+  <si>
+    <t>назва відділення</t>
+  </si>
+  <si>
+    <t>на Рік/Рікн.р</t>
+  </si>
+  <si>
+    <t>0 семестр</t>
+  </si>
+  <si>
+    <t>Студент: Ім'я Фамілія По-батькові (ГР-000)</t>
   </si>
 </sst>
 </file>
@@ -237,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -252,36 +261,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,296 +577,365 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="172" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="172" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="18" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="9" width="7.6640625" customWidth="1"/>
+    <col min="3" max="11" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+    <row r="1" spans="1:21" ht="28" customHeight="1">
+      <c r="A1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="1"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19" ht="18" customHeight="1">
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="3"/>
+    </row>
+    <row r="2" spans="1:21" ht="18" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="16" t="s">
+      <c r="H2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="8" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:21" ht="18" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1">
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:21" ht="18" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:21" ht="18" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="F5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1">
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1">
-      <c r="G6" s="9" t="s">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:21" ht="18" customHeight="1">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:21" ht="18" customHeight="1">
+      <c r="H7" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1">
-      <c r="A7" s="11" t="s">
+    <row r="8" spans="1:21" ht="18" customHeight="1">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:19" ht="18" customHeight="1">
-      <c r="A8" s="10" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="1:21" ht="18" customHeight="1">
+      <c r="A9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:21" ht="18" customHeight="1">
+      <c r="A10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:21" ht="18" customHeight="1">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="18" customHeight="1">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="18" customHeight="1">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="18" customHeight="1">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="18" customHeight="1">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="25" customHeight="1">
+      <c r="A16" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="34" customHeight="1">
+      <c r="A17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" ht="18" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" ht="18" customHeight="1">
+      <c r="A19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="1:11" ht="18" customHeight="1">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" ht="25" customHeight="1">
+      <c r="A21" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="34" customHeight="1">
+      <c r="A22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" ht="18" customHeight="1">
+      <c r="A23" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="1:11" ht="18" customHeight="1">
+      <c r="A24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="26" spans="1:11" ht="18" customHeight="1">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14" customHeight="1">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="20" customHeight="1">
-      <c r="A14" s="12" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+    </row>
+    <row r="28" spans="1:11" ht="11" customHeight="1">
+      <c r="D28" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" ht="31" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-    </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1">
-      <c r="A16" s="17" t="s">
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:11" ht="14" customHeight="1">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+    </row>
+    <row r="30" spans="1:11" ht="18" customHeight="1">
+      <c r="D30" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-    </row>
-    <row r="17" spans="1:9" ht="18" customHeight="1">
-      <c r="A17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="1:9" ht="18" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="1:9" ht="20" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="31" customHeight="1">
-      <c r="A20" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-    </row>
-    <row r="21" spans="1:9" ht="18" customHeight="1">
-      <c r="A21" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" ht="18" customHeight="1">
-      <c r="A22" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="24" spans="1:9" ht="18" customHeight="1">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14" customHeight="1">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="1:9" ht="11" customHeight="1">
-      <c r="D26" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" ht="14" customHeight="1">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="1:9" ht="18" customHeight="1">
-      <c r="D28" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-    </row>
-    <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="15" t="s">
-        <v>17</v>
-      </c>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="D27:I27"/>
+  <mergeCells count="12">
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A10:K10"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="I30:K30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294"/>

</xml_diff>